<commit_message>
made edits to grubert version of manuscript
</commit_message>
<xml_diff>
--- a/BMC_Genome_Biology_submission/main_tables/table1.xlsx
+++ b/BMC_Genome_Biology_submission/main_tables/table1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stili\Documents\TAD_predictive_modeling\Manuscript\Figures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stili\Documents\TAD_predictive_modeling\BMC_Genome_Biology_submission\main_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{78755075-09FD-41C3-B921-E1F94E6EC72C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31620252-D345-4285-9370-1A14221E972C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{4F6D0ACF-0DC0-4A5E-9E26-5F09F33B8575}"/>
+    <workbookView xWindow="-380" yWindow="555" windowWidth="19200" windowHeight="10380" xr2:uid="{4F6D0ACF-0DC0-4A5E-9E26-5F09F33B8575}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -36,9 +30,6 @@
     <t>Tool</t>
   </si>
   <si>
-    <t>Resolution</t>
-  </si>
-  <si>
     <t>Total number of called TADs/chromatin loops</t>
   </si>
   <si>
@@ -51,9 +42,6 @@
     <t>Class imbalance</t>
   </si>
   <si>
-    <t>ARROWHEAD</t>
-  </si>
-  <si>
     <t>5 kb</t>
   </si>
   <si>
@@ -69,7 +57,13 @@
     <t>100 kb</t>
   </si>
   <si>
-    <t>PEAKACHU</t>
+    <t>Arrowhead</t>
+  </si>
+  <si>
+    <t>Peakachu</t>
+  </si>
+  <si>
+    <t>Resolution/Bin size</t>
   </si>
 </sst>
 </file>
@@ -424,7 +418,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -434,27 +428,27 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>8052</v>
@@ -471,10 +465,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
       </c>
       <c r="C3">
         <v>7676</v>
@@ -491,10 +485,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C4">
         <v>4670</v>
@@ -511,10 +505,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5">
         <v>2349</v>
@@ -531,10 +525,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C6">
         <v>1031</v>
@@ -551,10 +545,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C7">
         <v>16185</v>

</xml_diff>